<commit_message>
Minor adjustments to mappings Added BurgelijkeStaat mapping
</commit_message>
<xml_diff>
--- a/Mappings/FunctionalOrMentalStatus - STU3.xlsx
+++ b/Mappings/FunctionalOrMentalStatus - STU3.xlsx
@@ -11,12 +11,12 @@
     <sheet name="StatusNaamCodelijst " sheetId="3" r:id="rId2"/>
     <sheet name="StatusWaardeCodelijst" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -54,9 +54,6 @@
     <t>RF</t>
   </si>
   <si>
-    <t>Observation.effectiveDateTime</t>
-  </si>
-  <si>
     <t>FunctioneleOfMentaleStatus</t>
   </si>
   <si>
@@ -184,6 +181,12 @@
   </si>
   <si>
     <t>ZIB-valueset can be used</t>
+  </si>
+  <si>
+    <t>Observation.effectivePeriod.start</t>
+  </si>
+  <si>
+    <t>Allow for an end time. (ZIB does not mention this)</t>
   </si>
 </sst>
 </file>
@@ -530,30 +533,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -563,6 +542,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -869,7 +872,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -889,15 +892,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
@@ -910,16 +913,16 @@
     </row>
     <row r="2" spans="1:12" ht="15">
       <c r="A2" s="3"/>
-      <c r="B2" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="33"/>
+      <c r="B2" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="37"/>
       <c r="J2" s="4" t="s">
         <v>5</v>
       </c>
@@ -940,8 +943,8 @@
         <v>8</v>
       </c>
       <c r="J3" s="9"/>
-      <c r="K3" s="38" t="s">
-        <v>54</v>
+      <c r="K3" s="30" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -950,12 +953,12 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="13"/>
@@ -963,10 +966,10 @@
         <v>8</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="35" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -975,12 +978,12 @@
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="13"/>
@@ -988,10 +991,10 @@
         <v>9</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="35" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -999,13 +1002,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="34"/>
+      <c r="C6" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="38"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="13"/>
@@ -1013,19 +1016,21 @@
         <v>9</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="25"/>
+        <v>55</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="10">
         <v>4</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
         <v>6</v>
@@ -1036,7 +1041,7 @@
         <v>7</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K7" s="25"/>
     </row>
@@ -1045,13 +1050,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="17"/>
-      <c r="C8" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="27"/>
+      <c r="C8" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="31"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="19"/>
@@ -1059,24 +1064,24 @@
         <v>11</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K8" s="26"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="K12" s="36"/>
-      <c r="L12" s="37"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="29"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="K15" s="37"/>
+      <c r="K15" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1108,130 +1113,130 @@
   <sheetData>
     <row r="3" spans="2:4">
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
         <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>26</v>
-      </c>
-      <c r="D21" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
         <v>37</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
         <v>25</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>26</v>
-      </c>
-      <c r="D28" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
         <v>41</v>
-      </c>
-      <c r="D29" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1256,130 +1261,130 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
         <v>25</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>26</v>
-      </c>
-      <c r="D20" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
         <v>37</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>26</v>
-      </c>
-      <c r="D27" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" t="s">
         <v>41</v>
-      </c>
-      <c r="D28" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>